<commit_message>
Upload current notes and screenshots.
</commit_message>
<xml_diff>
--- a/ScrumAge_SystemTestPlan.xlsx
+++ b/ScrumAge_SystemTestPlan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimmy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimmy\Documents\Scrumage\scrumage\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
   <si>
     <t xml:space="preserve">Test Scenario ID </t>
   </si>
@@ -204,9 +204,6 @@
     <t>Move node</t>
   </si>
   <si>
-    <t>1. Select pawn from pawn list. 2. Select location from drop down menu. 3. click move pawn button.</t>
-  </si>
-  <si>
     <t>front end, X</t>
   </si>
   <si>
@@ -229,6 +226,65 @@
   </si>
   <si>
     <t>Receive additional funds in label for player.</t>
+  </si>
+  <si>
+    <t>Gain pawn from interview in phase 2</t>
+  </si>
+  <si>
+    <t>Gain pawn from interview node in phase 2</t>
+  </si>
+  <si>
+    <t>1. Assign 2 pawns to node as TS03. 2. During phase 2 select interview from location drop down. 3. click Node Action.</t>
+  </si>
+  <si>
+    <t>2 of any type of pawn</t>
+  </si>
+  <si>
+    <t>Receive 3 pawns back to pawn list.</t>
+  </si>
+  <si>
+    <t>TS07</t>
+  </si>
+  <si>
+    <t>Increase budget</t>
+  </si>
+  <si>
+    <t>TC10</t>
+  </si>
+  <si>
+    <t>Budget increase</t>
+  </si>
+  <si>
+    <t>1. Assign 1 pawn to node as TS03. 2. During phase 2 select interview from location drop down. 3. Click node action</t>
+  </si>
+  <si>
+    <t>Budget increases by 1</t>
+  </si>
+  <si>
+    <t>1 of any type of pawn</t>
+  </si>
+  <si>
+    <t>1. Select pawn from pawn list. 
+2. Select location from drop down menu. 
+3. click move pawn button.</t>
+  </si>
+  <si>
+    <t>open help menu during play</t>
+  </si>
+  <si>
+    <t>1. Click help button_x000D_
+2. Help Menu opens_x000D_
+3. Click close button
+4.Help menu closes</t>
+  </si>
+  <si>
+    <t>tc06</t>
+  </si>
+  <si>
+    <t>Exit Game</t>
+  </si>
+  <si>
+    <t>exit game during play</t>
   </si>
 </sst>
 </file>
@@ -309,8 +365,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I10" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:I10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I13" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:I13"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Test Scenario ID "/>
     <tableColumn id="2" name="Test Scenario "/>
@@ -623,18 +679,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" customWidth="1"/>
     <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" customWidth="1"/>
@@ -764,81 +820,157 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>36</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>47</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>42</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
         <v>49</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="1" t="s">
+    </row>
+    <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
         <v>52</v>
       </c>
-      <c r="C9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="B12" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated system test plan for full phase coverage. Added meeting notes and trello screenshots.
</commit_message>
<xml_diff>
--- a/ScrumAge_SystemTestPlan.xlsx
+++ b/ScrumAge_SystemTestPlan.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="145">
   <si>
     <t xml:space="preserve">Test Scenario ID </t>
   </si>
@@ -169,9 +169,6 @@
     <t>Exit main menu</t>
   </si>
   <si>
-    <t>TC06</t>
-  </si>
-  <si>
     <t>exit main menu</t>
   </si>
   <si>
@@ -196,12 +193,6 @@
   </si>
   <si>
     <t>TC09</t>
-  </si>
-  <si>
-    <t>Move Node</t>
-  </si>
-  <si>
-    <t>Move node</t>
   </si>
   <si>
     <t>front end, X</t>
@@ -285,6 +276,225 @@
   </si>
   <si>
     <t>exit game during play</t>
+  </si>
+  <si>
+    <t>TS08</t>
+  </si>
+  <si>
+    <t>TC11</t>
+  </si>
+  <si>
+    <t>TS09</t>
+  </si>
+  <si>
+    <t>Move to Node</t>
+  </si>
+  <si>
+    <t>Move to node on board</t>
+  </si>
+  <si>
+    <t>Resolve Node</t>
+  </si>
+  <si>
+    <t>Resolve node to gain resource</t>
+  </si>
+  <si>
+    <t>1. Assign devs to nodes as TS05 2. Finish assigning all remaining developers to available nodes. 3. Choose node from drop down (ie. Requirements) 4. Click Node Action button</t>
+  </si>
+  <si>
+    <t>desired number of pawns, desired node</t>
+  </si>
+  <si>
+    <t>Resolve resource action, receive resource depending on roll on percentage.</t>
+  </si>
+  <si>
+    <t>Upgrade Pawn</t>
+  </si>
+  <si>
+    <t>Upgrade pawn from front/back end developer to full stack developer</t>
+  </si>
+  <si>
+    <t>1. Assign devs to nodes as TS05 2. Select Technical Hut location from drop down. 3. Select Move Pawn button. 4. Assign all other pawns to other nodes. 5. Once in phase 2 select technical hut from drop down menu. 6. Click Node Action Button</t>
+  </si>
+  <si>
+    <t>1 front/back end pawn, Technical Hut Node</t>
+  </si>
+  <si>
+    <t>Upgraded full stack developer added to pawn list.</t>
+  </si>
+  <si>
+    <t>Upgrade full stack pawn from front/back end developer to full stack developer</t>
+  </si>
+  <si>
+    <t>1. Assign full stack dev to nodes as TS05 2. Select Technical Hut location from drop down. 3. Select Move Pawn button. 4. Assign all other pawns to other nodes. 5. Once in phase 2 select technical hut from drop down menu. 6. Click Node Action Button</t>
+  </si>
+  <si>
+    <t>1 full stack developer, technical hut node</t>
+  </si>
+  <si>
+    <t>Error that full stack developer could not be upgraded further</t>
+  </si>
+  <si>
+    <t>Allowed player to assign full stack to technical hut Node</t>
+  </si>
+  <si>
+    <t>TS10</t>
+  </si>
+  <si>
+    <t>TC12</t>
+  </si>
+  <si>
+    <t>TC13</t>
+  </si>
+  <si>
+    <t>TS11</t>
+  </si>
+  <si>
+    <t>Gain card</t>
+  </si>
+  <si>
+    <t>Gain artifact or agility card by assigning pawn to node</t>
+  </si>
+  <si>
+    <t>1 pawn, any card node</t>
+  </si>
+  <si>
+    <t>Gain 1 card if enough resources present. Otherwise, receive no bonus and pawn returns to pawn list.</t>
+  </si>
+  <si>
+    <t>TS12</t>
+  </si>
+  <si>
+    <t>View Card details</t>
+  </si>
+  <si>
+    <t>TC15</t>
+  </si>
+  <si>
+    <t>TC14</t>
+  </si>
+  <si>
+    <t>Click "Card Info Label" to view card details</t>
+  </si>
+  <si>
+    <t>1. Once game board is displayed double click "Card info Label" 2. Click ok. Alt 2. Click X in upper right hand corner of pop up window.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View card details window and verify information. </t>
+  </si>
+  <si>
+    <t>Determined to be a strategy mechanic to block others from assigning pawn.</t>
+  </si>
+  <si>
+    <t>TS13</t>
+  </si>
+  <si>
+    <t>Roll Rice</t>
+  </si>
+  <si>
+    <t>TC16</t>
+  </si>
+  <si>
+    <t>Roll set number of dice and find result</t>
+  </si>
+  <si>
+    <t>1. Once game board is displayed, select number of dice from drop down menu above help button. 2. Click Roll dice button.</t>
+  </si>
+  <si>
+    <t>View result of rolled dice in Sprint Log.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TS14 </t>
+  </si>
+  <si>
+    <t>Test button</t>
+  </si>
+  <si>
+    <t>Press test button to gain resources</t>
+  </si>
+  <si>
+    <t>1. Once game board is displayed, press Test Button.</t>
+  </si>
+  <si>
+    <t>Gain 1000 resources of each type and 6 cards.</t>
+  </si>
+  <si>
+    <t>View current card details</t>
+  </si>
+  <si>
+    <t>View current card details in inventory</t>
+  </si>
+  <si>
+    <t>1. Once received card in TS11. 2. Click card in inventory display.</t>
+  </si>
+  <si>
+    <t>Create window to view card details.</t>
+  </si>
+  <si>
+    <t>TS15</t>
+  </si>
+  <si>
+    <t>TC17</t>
+  </si>
+  <si>
+    <t>TC18</t>
+  </si>
+  <si>
+    <t>TS16</t>
+  </si>
+  <si>
+    <t>Progress to phase 3</t>
+  </si>
+  <si>
+    <t>TC19</t>
+  </si>
+  <si>
+    <t>Progress game past phase 2 into phase 3</t>
+  </si>
+  <si>
+    <t>1. Assign pawn to node as TS05. 2. Select either Agility 1-4 or Artifact 1-4 from drop down. 3. Select Move Pawn button. 4. Add all remaining devs to nodes. 5. Select card location from location drop down. 6. Click Node Action Button</t>
+  </si>
+  <si>
+    <t>Progress to phase 2</t>
+  </si>
+  <si>
+    <t>Progress game past phase 1 into phase 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Assign all pawns to nodes in TS05 </t>
+  </si>
+  <si>
+    <t>Auto moved to phase 2 and able to resolve nodes into resources or upgrades.</t>
+  </si>
+  <si>
+    <t>TS17</t>
+  </si>
+  <si>
+    <t>TC20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. move to phase 2 in TS16. 2. For each pawn at each node, the location must be chosen from drop down menu. 3. Click Node Action Button. </t>
+  </si>
+  <si>
+    <t>pop up box stating phase 2 done.</t>
+  </si>
+  <si>
+    <t>TS18</t>
+  </si>
+  <si>
+    <t>Progress to phase 1</t>
+  </si>
+  <si>
+    <t>TC21</t>
+  </si>
+  <si>
+    <t>Progress game from phase 3 to phase 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Move to phase 3 in TS17. 2. Click Trade for Funds button for each player. </t>
+  </si>
+  <si>
+    <t>Decrements funds count by dev payment count and moves to phase 1 again.</t>
   </si>
 </sst>
 </file>
@@ -326,17 +536,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -365,18 +595,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I13" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:I13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I24" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:I24"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Test Scenario ID "/>
-    <tableColumn id="2" name="Test Scenario "/>
+    <tableColumn id="2" name="Test Scenario " dataDxfId="0"/>
     <tableColumn id="3" name="Test Case ID "/>
-    <tableColumn id="4" name="Test Case name"/>
-    <tableColumn id="5" name="Test Steps" dataDxfId="1"/>
-    <tableColumn id="6" name="Test Data"/>
-    <tableColumn id="7" name="Expected Outcome" dataDxfId="0"/>
-    <tableColumn id="8" name="Actual Outcome"/>
-    <tableColumn id="9" name="Result"/>
+    <tableColumn id="4" name="Test Case name" dataDxfId="6"/>
+    <tableColumn id="5" name="Test Steps" dataDxfId="5"/>
+    <tableColumn id="6" name="Test Data" dataDxfId="4"/>
+    <tableColumn id="7" name="Expected Outcome" dataDxfId="3"/>
+    <tableColumn id="8" name="Actual Outcome" dataDxfId="2"/>
+    <tableColumn id="9" name="Result" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -679,50 +909,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
-    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -730,247 +961,534 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
-        <v>73</v>
+      <c r="B8" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s">
-        <v>74</v>
+        <v>41</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="F11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" t="s">
-        <v>55</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="G12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B13" t="s">
+      <c r="E13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C13" t="s">
+      <c r="F13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="224.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>